<commit_message>
7/10/20: ran scrape and analysis
</commit_message>
<xml_diff>
--- a/combined-datasets/demographics.xlsx
+++ b/combined-datasets/demographics.xlsx
@@ -10329,6 +10329,266 @@
         <v>0</v>
       </c>
     </row>
+    <row r="496">
+      <c r="A496" s="1" t="n">
+        <v>44022</v>
+      </c>
+      <c r="B496" t="s">
+        <v>6</v>
+      </c>
+      <c r="C496" t="n">
+        <v>461</v>
+      </c>
+      <c r="D496" t="n">
+        <v>1.8620243962</v>
+      </c>
+      <c r="E496" t="n">
+        <v>0</v>
+      </c>
+      <c r="F496" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" s="1" t="n">
+        <v>44022</v>
+      </c>
+      <c r="B497" t="s">
+        <v>7</v>
+      </c>
+      <c r="C497" t="n">
+        <v>1198</v>
+      </c>
+      <c r="D497" t="n">
+        <v>4.8388399709</v>
+      </c>
+      <c r="E497" t="n">
+        <v>0</v>
+      </c>
+      <c r="F497" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" s="1" t="n">
+        <v>44022</v>
+      </c>
+      <c r="B498" t="s">
+        <v>8</v>
+      </c>
+      <c r="C498" t="n">
+        <v>4538</v>
+      </c>
+      <c r="D498" t="n">
+        <v>18.329428871</v>
+      </c>
+      <c r="E498" t="n">
+        <v>4</v>
+      </c>
+      <c r="F498" t="n">
+        <v>0.5633802817</v>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" s="1" t="n">
+        <v>44022</v>
+      </c>
+      <c r="B499" t="s">
+        <v>9</v>
+      </c>
+      <c r="C499" t="n">
+        <v>4577</v>
+      </c>
+      <c r="D499" t="n">
+        <v>18.486953712</v>
+      </c>
+      <c r="E499" t="n">
+        <v>12</v>
+      </c>
+      <c r="F499" t="n">
+        <v>1.6901408451</v>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" s="1" t="n">
+        <v>44022</v>
+      </c>
+      <c r="B500" t="s">
+        <v>10</v>
+      </c>
+      <c r="C500" t="n">
+        <v>4407</v>
+      </c>
+      <c r="D500" t="n">
+        <v>17.800306971</v>
+      </c>
+      <c r="E500" t="n">
+        <v>26</v>
+      </c>
+      <c r="F500" t="n">
+        <v>3.661971831</v>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" s="1" t="n">
+        <v>44022</v>
+      </c>
+      <c r="B501" t="s">
+        <v>11</v>
+      </c>
+      <c r="C501" t="n">
+        <v>4146</v>
+      </c>
+      <c r="D501" t="n">
+        <v>16.74610227</v>
+      </c>
+      <c r="E501" t="n">
+        <v>75</v>
+      </c>
+      <c r="F501" t="n">
+        <v>10.563380282</v>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" s="1" t="n">
+        <v>44022</v>
+      </c>
+      <c r="B502" t="s">
+        <v>12</v>
+      </c>
+      <c r="C502" t="n">
+        <v>1650</v>
+      </c>
+      <c r="D502" t="n">
+        <v>6.6645124808</v>
+      </c>
+      <c r="E502" t="n">
+        <v>71</v>
+      </c>
+      <c r="F502" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" s="1" t="n">
+        <v>44022</v>
+      </c>
+      <c r="B503" t="s">
+        <v>13</v>
+      </c>
+      <c r="C503" t="n">
+        <v>1196</v>
+      </c>
+      <c r="D503" t="n">
+        <v>4.830761774</v>
+      </c>
+      <c r="E503" t="n">
+        <v>82</v>
+      </c>
+      <c r="F503" t="n">
+        <v>11.549295775</v>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" s="1" t="n">
+        <v>44022</v>
+      </c>
+      <c r="B504" t="s">
+        <v>14</v>
+      </c>
+      <c r="C504" t="n">
+        <v>778</v>
+      </c>
+      <c r="D504" t="n">
+        <v>3.1424186122</v>
+      </c>
+      <c r="E504" t="n">
+        <v>78</v>
+      </c>
+      <c r="F504" t="n">
+        <v>10.985915493</v>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" s="1" t="n">
+        <v>44022</v>
+      </c>
+      <c r="B505" t="s">
+        <v>15</v>
+      </c>
+      <c r="C505" t="n">
+        <v>586</v>
+      </c>
+      <c r="D505" t="n">
+        <v>2.3669117053</v>
+      </c>
+      <c r="E505" t="n">
+        <v>80</v>
+      </c>
+      <c r="F505" t="n">
+        <v>11.267605634</v>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" s="1" t="n">
+        <v>44022</v>
+      </c>
+      <c r="B506" t="s">
+        <v>16</v>
+      </c>
+      <c r="C506" t="n">
+        <v>1103</v>
+      </c>
+      <c r="D506" t="n">
+        <v>4.455125616</v>
+      </c>
+      <c r="E506" t="n">
+        <v>282</v>
+      </c>
+      <c r="F506" t="n">
+        <v>39.718309859</v>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" s="1" t="n">
+        <v>44022</v>
+      </c>
+      <c r="B507" t="s">
+        <v>17</v>
+      </c>
+      <c r="C507" t="n">
+        <v>102</v>
+      </c>
+      <c r="D507" t="n">
+        <v>0.4119880443</v>
+      </c>
+      <c r="E507" t="n">
+        <v>0</v>
+      </c>
+      <c r="F507" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" s="1" t="n">
+        <v>44022</v>
+      </c>
+      <c r="B508" t="s">
+        <v>18</v>
+      </c>
+      <c r="C508" t="n">
+        <v>16</v>
+      </c>
+      <c r="D508" t="n">
+        <v>0.0646255756</v>
+      </c>
+      <c r="E508" t="n">
+        <v>0</v>
+      </c>
+      <c r="F508" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -12643,6 +12903,66 @@
         <v>0.0042674253200569</v>
       </c>
     </row>
+    <row r="116">
+      <c r="A116" s="1" t="n">
+        <v>44022</v>
+      </c>
+      <c r="B116" t="s">
+        <v>19</v>
+      </c>
+      <c r="C116" t="n">
+        <v>11928</v>
+      </c>
+      <c r="D116" t="n">
+        <v>48.178366589</v>
+      </c>
+      <c r="E116" t="n">
+        <v>292</v>
+      </c>
+      <c r="F116" t="n">
+        <v>41.126760563</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="n">
+        <v>44022</v>
+      </c>
+      <c r="B117" t="s">
+        <v>20</v>
+      </c>
+      <c r="C117" t="n">
+        <v>12560</v>
+      </c>
+      <c r="D117" t="n">
+        <v>50.731076824</v>
+      </c>
+      <c r="E117" t="n">
+        <v>415</v>
+      </c>
+      <c r="F117" t="n">
+        <v>58.450704225</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="n">
+        <v>44022</v>
+      </c>
+      <c r="B118" t="s">
+        <v>18</v>
+      </c>
+      <c r="C118" t="n">
+        <v>270</v>
+      </c>
+      <c r="D118" t="n">
+        <v>1.0905565878</v>
+      </c>
+      <c r="E118" t="n">
+        <v>3</v>
+      </c>
+      <c r="F118" t="n">
+        <v>0.4225352113</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -17117,6 +17437,126 @@
         <v>0.432432432432432</v>
       </c>
     </row>
+    <row r="224">
+      <c r="A224" s="1" t="n">
+        <v>44022</v>
+      </c>
+      <c r="B224" t="s">
+        <v>21</v>
+      </c>
+      <c r="C224" t="n">
+        <v>640</v>
+      </c>
+      <c r="D224" t="n">
+        <v>2.5850230229</v>
+      </c>
+      <c r="E224" t="n">
+        <v>14</v>
+      </c>
+      <c r="F224" t="n">
+        <v>1.9718309859</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="1" t="n">
+        <v>44022</v>
+      </c>
+      <c r="B225" t="s">
+        <v>22</v>
+      </c>
+      <c r="C225" t="n">
+        <v>2851</v>
+      </c>
+      <c r="D225" t="n">
+        <v>11.515469747</v>
+      </c>
+      <c r="E225" t="n">
+        <v>91</v>
+      </c>
+      <c r="F225" t="n">
+        <v>12.816901408</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="1" t="n">
+        <v>44022</v>
+      </c>
+      <c r="B226" t="s">
+        <v>23</v>
+      </c>
+      <c r="C226" t="n">
+        <v>9712</v>
+      </c>
+      <c r="D226" t="n">
+        <v>39.227724372</v>
+      </c>
+      <c r="E226" t="n">
+        <v>205</v>
+      </c>
+      <c r="F226" t="n">
+        <v>28.873239437</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="1" t="n">
+        <v>44022</v>
+      </c>
+      <c r="B227" t="s">
+        <v>24</v>
+      </c>
+      <c r="C227" t="n">
+        <v>132</v>
+      </c>
+      <c r="D227" t="n">
+        <v>0.5331609985</v>
+      </c>
+      <c r="E227" t="n">
+        <v>1</v>
+      </c>
+      <c r="F227" t="n">
+        <v>0.1408450704</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="1" t="n">
+        <v>44022</v>
+      </c>
+      <c r="B228" t="s">
+        <v>18</v>
+      </c>
+      <c r="C228" t="n">
+        <v>5234</v>
+      </c>
+      <c r="D228" t="n">
+        <v>21.140641409</v>
+      </c>
+      <c r="E228" t="n">
+        <v>90</v>
+      </c>
+      <c r="F228" t="n">
+        <v>12.676056338</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="1" t="n">
+        <v>44022</v>
+      </c>
+      <c r="B229" t="s">
+        <v>25</v>
+      </c>
+      <c r="C229" t="n">
+        <v>6189</v>
+      </c>
+      <c r="D229" t="n">
+        <v>24.997980451</v>
+      </c>
+      <c r="E229" t="n">
+        <v>309</v>
+      </c>
+      <c r="F229" t="n">
+        <v>43.521126761</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>